<commit_message>
customizable configuration_item column name
</commit_message>
<xml_diff>
--- a/examples/files/data.xlsx
+++ b/examples/files/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\go\src\terraform-provider-config\examples\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariel/Documents/repos/go/src/terraform-provider-config/examples/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7069F29-A351-428F-AD4D-F76EEEE5FFA9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398ED418-2ADA-3340-B6A3-21C0163CF6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6850" xr2:uid="{B0AD3E86-2D5D-41DA-902C-D5987C5C163C}"/>
+    <workbookView xWindow="-27160" yWindow="5500" windowWidth="19200" windowHeight="12080" xr2:uid="{B0AD3E86-2D5D-41DA-902C-D5987C5C163C}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>configuration_item</t>
   </si>
@@ -45,9 +45,6 @@
     <t>attr3</t>
   </si>
   <si>
-    <t>attr4</t>
-  </si>
-  <si>
     <t>attr5</t>
   </si>
   <si>
@@ -109,6 +106,15 @@
   </si>
   <si>
     <t>"1,2,3,4"</t>
+  </si>
+  <si>
+    <t>m_mymap</t>
+  </si>
+  <si>
+    <t>t_test</t>
+  </si>
+  <si>
+    <t>hello</t>
   </si>
 </sst>
 </file>
@@ -460,18 +466,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09A65D6-13F4-4F11-B421-E0769E60F1F7}">
-  <dimension ref="B1:L4"/>
+  <dimension ref="B1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -485,62 +491,68 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2">
         <v>3.14</v>
       </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -549,33 +561,33 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3">
         <v>200</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3">
         <v>4.1550000000000002</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4">
         <v>1</v>

</xml_diff>

<commit_message>
add new parameter 'orientation' to cater vertical data types
</commit_message>
<xml_diff>
--- a/examples/files/data.xlsx
+++ b/examples/files/data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariel/Documents/repos/go/src/terraform-provider-config/examples/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D394AD2-D11B-7E49-BE1C-6BDB1D2D2A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709203C7-634B-F647-A5D7-F73A6E1F547C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27160" yWindow="5500" windowWidth="19200" windowHeight="12080" xr2:uid="{B0AD3E86-2D5D-41DA-902C-D5987C5C163C}"/>
+    <workbookView xWindow="12700" yWindow="4600" windowWidth="19200" windowHeight="12080" activeTab="1" xr2:uid="{B0AD3E86-2D5D-41DA-902C-D5987C5C163C}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
+    <sheet name="Vert" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>configuration_item</t>
   </si>
@@ -115,16 +116,40 @@
   </si>
   <si>
     <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>value1</t>
+  </si>
+  <si>
+    <t>value2</t>
+  </si>
+  <si>
+    <t>value3</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>cidr_block</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -468,7 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09A65D6-13F4-4F11-B421-E0769E60F1F7}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -600,4 +625,44 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A86D689-62A5-2C4B-BADF-72219E6A3529}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>